<commit_message>
sensor, leds, y mapeo 10/10
</commit_message>
<xml_diff>
--- a/logica_combinatoria_Tablas.xlsx
+++ b/logica_combinatoria_Tablas.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MRR79\Documents\P1-logica-combinatoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43AB607-C890-450D-9699-FB8273E198FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FC0F48C-521E-433B-9A8C-E19583ACF5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="deco" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="deco" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
   <si>
     <t>A</t>
   </si>
@@ -234,6 +236,30 @@
   </si>
   <si>
     <t xml:space="preserve">sn74hc08n </t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>xreves</t>
+  </si>
+  <si>
+    <t>seccion</t>
+  </si>
+  <si>
+    <t>pin 10</t>
+  </si>
+  <si>
+    <t>pin 11</t>
+  </si>
+  <si>
+    <t>pin 12</t>
+  </si>
+  <si>
+    <t>si</t>
   </si>
 </sst>
 </file>
@@ -389,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -554,11 +580,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -653,6 +688,27 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -670,12 +726,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,16 +799,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>354135</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114860</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>67164</xdr:rowOff>
+      <xdr:rowOff>168396</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>6106</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>170962</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>374223</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>14513</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -773,8 +823,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5238750" y="696058"/>
-          <a:ext cx="3926010" cy="1898894"/>
+          <a:off x="8618338" y="3012092"/>
+          <a:ext cx="3903711" cy="1907566"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1235,13 +1285,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="97" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="69" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
         <v>42</v>
       </c>
@@ -1258,7 +1308,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="32">
         <v>0</v>
       </c>
@@ -1275,7 +1325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="32">
         <v>1</v>
       </c>
@@ -1292,7 +1342,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="32">
         <v>2</v>
       </c>
@@ -1309,7 +1359,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="32">
         <v>3</v>
       </c>
@@ -1326,7 +1376,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="32">
         <v>4</v>
       </c>
@@ -1343,7 +1393,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="32">
         <v>5</v>
       </c>
@@ -1360,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="32">
         <v>6</v>
       </c>
@@ -1377,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="32">
         <v>7</v>
       </c>
@@ -1394,21 +1444,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="1:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="15"/>
-      <c r="B15" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="52" t="s">
+      <c r="B15" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="46" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="17" t="s">
@@ -1421,17 +1471,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="18">
         <v>0</v>
       </c>
-      <c r="B16" s="53">
-        <v>0</v>
-      </c>
-      <c r="C16" s="53">
-        <v>0</v>
-      </c>
-      <c r="D16" s="53">
+      <c r="B16" s="47">
+        <v>0</v>
+      </c>
+      <c r="C16" s="47">
+        <v>0</v>
+      </c>
+      <c r="D16" s="47">
         <v>0</v>
       </c>
       <c r="E16" s="15">
@@ -1442,19 +1492,22 @@
       </c>
       <c r="G16" s="15">
         <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="18">
         <v>1</v>
       </c>
-      <c r="B17" s="53">
-        <v>0</v>
-      </c>
-      <c r="C17" s="53">
-        <v>0</v>
-      </c>
-      <c r="D17" s="53">
+      <c r="B17" s="47">
+        <v>0</v>
+      </c>
+      <c r="C17" s="47">
+        <v>0</v>
+      </c>
+      <c r="D17" s="47">
         <v>1</v>
       </c>
       <c r="E17" s="15">
@@ -1465,19 +1518,22 @@
       </c>
       <c r="G17" s="15">
         <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="18">
         <v>2</v>
       </c>
-      <c r="B18" s="53">
-        <v>0</v>
-      </c>
-      <c r="C18" s="53">
-        <v>1</v>
-      </c>
-      <c r="D18" s="53">
+      <c r="B18" s="47">
+        <v>0</v>
+      </c>
+      <c r="C18" s="47">
+        <v>1</v>
+      </c>
+      <c r="D18" s="47">
         <v>1</v>
       </c>
       <c r="E18" s="15">
@@ -1487,6 +1543,18 @@
         <v>0</v>
       </c>
       <c r="G18" s="15">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" s="48">
+        <v>1</v>
+      </c>
+      <c r="J18" s="48">
+        <v>1</v>
+      </c>
+      <c r="K18" s="48">
         <v>1</v>
       </c>
     </row>
@@ -1494,13 +1562,13 @@
       <c r="A19" s="18">
         <v>3</v>
       </c>
-      <c r="B19" s="53">
-        <v>0</v>
-      </c>
-      <c r="C19" s="53">
-        <v>1</v>
-      </c>
-      <c r="D19" s="53">
+      <c r="B19" s="47">
+        <v>0</v>
+      </c>
+      <c r="C19" s="47">
+        <v>1</v>
+      </c>
+      <c r="D19" s="47">
         <v>0</v>
       </c>
       <c r="E19" s="15">
@@ -1511,19 +1579,22 @@
       </c>
       <c r="G19" s="15">
         <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="18">
         <v>4</v>
       </c>
-      <c r="B20" s="53">
-        <v>1</v>
-      </c>
-      <c r="C20" s="53">
-        <v>1</v>
-      </c>
-      <c r="D20" s="53">
+      <c r="B20" s="47">
+        <v>1</v>
+      </c>
+      <c r="C20" s="47">
+        <v>1</v>
+      </c>
+      <c r="D20" s="47">
         <v>0</v>
       </c>
       <c r="E20" s="15">
@@ -1534,19 +1605,22 @@
       </c>
       <c r="G20" s="15">
         <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="18">
         <v>5</v>
       </c>
-      <c r="B21" s="53">
-        <v>1</v>
-      </c>
-      <c r="C21" s="53">
-        <v>1</v>
-      </c>
-      <c r="D21" s="53">
+      <c r="B21" s="47">
+        <v>1</v>
+      </c>
+      <c r="C21" s="47">
+        <v>1</v>
+      </c>
+      <c r="D21" s="47">
         <v>1</v>
       </c>
       <c r="E21" s="15">
@@ -1557,19 +1631,31 @@
       </c>
       <c r="G21" s="15">
         <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="48">
+        <v>1</v>
+      </c>
+      <c r="J21" s="48">
+        <v>1</v>
+      </c>
+      <c r="K21" s="48">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="18">
         <v>6</v>
       </c>
-      <c r="B22" s="53">
-        <v>1</v>
-      </c>
-      <c r="C22" s="53">
-        <v>0</v>
-      </c>
-      <c r="D22" s="53">
+      <c r="B22" s="47">
+        <v>1</v>
+      </c>
+      <c r="C22" s="47">
+        <v>0</v>
+      </c>
+      <c r="D22" s="47">
         <v>1</v>
       </c>
       <c r="E22" s="15">
@@ -1580,19 +1666,22 @@
       </c>
       <c r="G22" s="15">
         <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="18">
         <v>7</v>
       </c>
-      <c r="B23" s="53">
-        <v>1</v>
-      </c>
-      <c r="C23" s="53">
-        <v>0</v>
-      </c>
-      <c r="D23" s="53">
+      <c r="B23" s="47">
+        <v>1</v>
+      </c>
+      <c r="C23" s="47">
+        <v>0</v>
+      </c>
+      <c r="D23" s="47">
         <v>0</v>
       </c>
       <c r="E23" s="15">
@@ -1604,13 +1693,16 @@
       <c r="G23" s="15">
         <v>0</v>
       </c>
+      <c r="H23" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
     </row>
     <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="30" t="s">
@@ -1636,10 +1728,10 @@
       <c r="H28" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="J28" s="50" t="s">
+      <c r="J28" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="K28" s="50"/>
+      <c r="K28" s="57"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B29" s="8">
@@ -1666,10 +1758,10 @@
       <c r="K29" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="L29" s="47" t="s">
+      <c r="L29" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="M29" s="48" t="s">
+      <c r="M29" s="55" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1695,8 +1787,8 @@
       <c r="K30" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="L30" s="47"/>
-      <c r="M30" s="48"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="55"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B31" s="1"/>
@@ -1734,10 +1826,10 @@
       <c r="H34" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="J34" s="50" t="s">
+      <c r="J34" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="K34" s="50"/>
+      <c r="K34" s="57"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B35" s="8">
@@ -1806,10 +1898,10 @@
       <c r="H40" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="L40" s="51" t="s">
+      <c r="L40" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="M40" s="51"/>
+      <c r="M40" s="58"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B41" s="8">
@@ -1827,11 +1919,11 @@
       <c r="F41" s="2">
         <v>0</v>
       </c>
-      <c r="H41" s="46" t="s">
+      <c r="H41" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="I41" s="46"/>
-      <c r="J41" s="46"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="53"/>
       <c r="L41" s="19" t="s">
         <v>29</v>
       </c>
@@ -2658,11 +2750,358 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3AB901-A249-4E01-9C77-28278758AC46}">
+  <dimension ref="A1:M26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="15"/>
+      <c r="B1" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="18">
+        <v>0</v>
+      </c>
+      <c r="B2" s="47">
+        <v>0</v>
+      </c>
+      <c r="C2" s="47">
+        <v>0</v>
+      </c>
+      <c r="D2" s="47">
+        <v>0</v>
+      </c>
+      <c r="E2" s="15">
+        <v>0</v>
+      </c>
+      <c r="F2" s="15">
+        <v>1</v>
+      </c>
+      <c r="G2" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="18">
+        <v>1</v>
+      </c>
+      <c r="B3" s="47">
+        <v>0</v>
+      </c>
+      <c r="C3" s="47">
+        <v>0</v>
+      </c>
+      <c r="D3" s="47">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15">
+        <v>0</v>
+      </c>
+      <c r="G3" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="18">
+        <v>2</v>
+      </c>
+      <c r="B4" s="47">
+        <v>0</v>
+      </c>
+      <c r="C4" s="47">
+        <v>1</v>
+      </c>
+      <c r="D4" s="47">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15">
+        <v>1</v>
+      </c>
+      <c r="F4" s="15">
+        <v>0</v>
+      </c>
+      <c r="G4" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="18">
+        <v>3</v>
+      </c>
+      <c r="B5" s="47">
+        <v>0</v>
+      </c>
+      <c r="C5" s="47">
+        <v>1</v>
+      </c>
+      <c r="D5" s="47">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15">
+        <v>1</v>
+      </c>
+      <c r="F5" s="15">
+        <v>1</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="18">
+        <v>4</v>
+      </c>
+      <c r="B6" s="47">
+        <v>1</v>
+      </c>
+      <c r="C6" s="47">
+        <v>1</v>
+      </c>
+      <c r="D6" s="47">
+        <v>0</v>
+      </c>
+      <c r="E6" s="15">
+        <v>1</v>
+      </c>
+      <c r="F6" s="15">
+        <v>1</v>
+      </c>
+      <c r="G6" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="18">
+        <v>5</v>
+      </c>
+      <c r="B7" s="47">
+        <v>1</v>
+      </c>
+      <c r="C7" s="47">
+        <v>1</v>
+      </c>
+      <c r="D7" s="47">
+        <v>1</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0</v>
+      </c>
+      <c r="F7" s="15">
+        <v>0</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="18">
+        <v>6</v>
+      </c>
+      <c r="B8" s="47">
+        <v>1</v>
+      </c>
+      <c r="C8" s="47">
+        <v>0</v>
+      </c>
+      <c r="D8" s="47">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0</v>
+      </c>
+      <c r="F8" s="15">
+        <v>0</v>
+      </c>
+      <c r="G8" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="18">
+        <v>7</v>
+      </c>
+      <c r="B9" s="47">
+        <v>1</v>
+      </c>
+      <c r="C9" s="47">
+        <v>0</v>
+      </c>
+      <c r="D9" s="47">
+        <v>0</v>
+      </c>
+      <c r="E9" s="15">
+        <v>0</v>
+      </c>
+      <c r="F9" s="15">
+        <v>1</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="10:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="18" spans="10:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J18" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18" s="50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="10:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J19" s="51">
+        <v>0</v>
+      </c>
+      <c r="K19" s="52">
+        <v>0</v>
+      </c>
+      <c r="L19" s="52">
+        <v>0</v>
+      </c>
+      <c r="M19" s="52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="10:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J20" s="51">
+        <v>1</v>
+      </c>
+      <c r="K20" s="52">
+        <v>0</v>
+      </c>
+      <c r="L20" s="52">
+        <v>0</v>
+      </c>
+      <c r="M20" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="10:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J21" s="51">
+        <v>2</v>
+      </c>
+      <c r="K21" s="52">
+        <v>0</v>
+      </c>
+      <c r="L21" s="52">
+        <v>1</v>
+      </c>
+      <c r="M21" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="10:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J22" s="51">
+        <v>3</v>
+      </c>
+      <c r="K22" s="52">
+        <v>0</v>
+      </c>
+      <c r="L22" s="52">
+        <v>1</v>
+      </c>
+      <c r="M22" s="52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="10:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J23" s="51">
+        <v>4</v>
+      </c>
+      <c r="K23" s="52">
+        <v>1</v>
+      </c>
+      <c r="L23" s="52">
+        <v>1</v>
+      </c>
+      <c r="M23" s="52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="10:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J24" s="51">
+        <v>5</v>
+      </c>
+      <c r="K24" s="52">
+        <v>1</v>
+      </c>
+      <c r="L24" s="52">
+        <v>1</v>
+      </c>
+      <c r="M24" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="10:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J25" s="51">
+        <v>6</v>
+      </c>
+      <c r="K25" s="52">
+        <v>1</v>
+      </c>
+      <c r="L25" s="52">
+        <v>0</v>
+      </c>
+      <c r="M25" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="10:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J26" s="51">
+        <v>7</v>
+      </c>
+      <c r="K26" s="52">
+        <v>1</v>
+      </c>
+      <c r="L26" s="52">
+        <v>0</v>
+      </c>
+      <c r="M26" s="52">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E67AD92-ED75-4DDC-A80D-FF82C2AC139A}">
-  <dimension ref="C8:M17"/>
+  <dimension ref="C8:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" zoomScale="130" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="B20" zoomScale="85" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2853,7 +3292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C17" s="44">
         <v>7</v>
       </c>
@@ -2867,6 +3306,136 @@
         <v>0</v>
       </c>
       <c r="G17" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E21" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E22" s="47">
+        <v>0</v>
+      </c>
+      <c r="F22" s="47">
+        <v>0</v>
+      </c>
+      <c r="G22" s="47">
+        <v>0</v>
+      </c>
+      <c r="H22" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E23" s="47">
+        <v>0</v>
+      </c>
+      <c r="F23" s="47">
+        <v>0</v>
+      </c>
+      <c r="G23" s="47">
+        <v>1</v>
+      </c>
+      <c r="H23" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E24" s="47">
+        <v>0</v>
+      </c>
+      <c r="F24" s="47">
+        <v>1</v>
+      </c>
+      <c r="G24" s="47">
+        <v>1</v>
+      </c>
+      <c r="H24" s="45">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E25" s="47">
+        <v>0</v>
+      </c>
+      <c r="F25" s="47">
+        <v>1</v>
+      </c>
+      <c r="G25" s="47">
+        <v>0</v>
+      </c>
+      <c r="H25" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E26" s="47">
+        <v>1</v>
+      </c>
+      <c r="F26" s="47">
+        <v>1</v>
+      </c>
+      <c r="G26" s="47">
+        <v>0</v>
+      </c>
+      <c r="H26" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E27" s="47">
+        <v>1</v>
+      </c>
+      <c r="F27" s="47">
+        <v>1</v>
+      </c>
+      <c r="G27" s="47">
+        <v>1</v>
+      </c>
+      <c r="H27" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E28" s="47">
+        <v>1</v>
+      </c>
+      <c r="F28" s="47">
+        <v>0</v>
+      </c>
+      <c r="G28" s="47">
+        <v>1</v>
+      </c>
+      <c r="H28" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E29" s="47">
+        <v>1</v>
+      </c>
+      <c r="F29" s="47">
+        <v>0</v>
+      </c>
+      <c r="G29" s="47">
+        <v>0</v>
+      </c>
+      <c r="H29" s="45">
         <v>1</v>
       </c>
     </row>
@@ -2876,6 +3445,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010094164D9811B23F4CA48C9254C527A113" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c98d7874cdf8ebf6adb2e4e309a14965">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b5d40255-19c5-496d-8152-a83d27b620bd" xmlns:ns4="ca3c2452-e284-49b8-b0a6-baec811be044" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="195d962093fd1c8664e7783ab7efd8ad" ns3:_="" ns4:_="">
     <xsd:import namespace="b5d40255-19c5-496d-8152-a83d27b620bd"/>
@@ -3122,7 +3700,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="b5d40255-19c5-496d-8152-a83d27b620bd" xsi:nil="true"/>
@@ -3130,16 +3708,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DC9736B-9418-40FA-A971-0FE8339CEB0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE96E676-8070-4258-B589-FFC8718B1BC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3158,7 +3735,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3CB7A86-3DB2-49D4-BE07-2DC6D11FBB5D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3173,12 +3750,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DC9736B-9418-40FA-A971-0FE8339CEB0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>